<commit_message>
atualizção ata dia 16/08/2023
</commit_message>
<xml_diff>
--- a/documentos/ata de reuniões.xlsx
+++ b/documentos/ata de reuniões.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\again\OneDrive\Documentos\faculdade\2ºSemestre\Sprint 1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AE6D49-82F7-4FAA-B4EF-2A32CCFF6F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AD0F1862-5E9D-4B18-95FC-025C3E4A5399}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Nome Do Projeto</t>
   </si>
@@ -66,12 +60,15 @@
   </si>
   <si>
     <t>Definição das Tarefas para a Semana</t>
+  </si>
+  <si>
+    <t>Produção na aula de PI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,7 +185,7 @@
         <xdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41122CF9-0C6D-46F7-E5B2-F7A9A99E0A3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41122CF9-0C6D-46F7-E5B2-F7A9A99E0A3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -256,6 +253,74 @@
             <a:t>Site -  one page</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38877</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>64796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2293775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1632857</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41122CF9-0C6D-46F7-E5B2-F7A9A99E0A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4072423" y="2727908"/>
+          <a:ext cx="2207273" cy="1568061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>Nos juntamos em grupo na aula. Separamos tarefas para tofods do grupo, onde alguns codaram e outros fizeram a proto-persona e o mind-Map . Conversamos sobre possiveis itens na area de usuário do protótipo</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -553,33 +618,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69104527-B39B-47BF-A58E-D49200CAEA07}">
-  <dimension ref="B2:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" customWidth="1"/>
-    <col min="4" max="4" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -589,8 +655,11 @@
       <c r="D3" s="5">
         <v>45147</v>
       </c>
+      <c r="E3" s="5">
+        <v>45154</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -600,15 +669,19 @@
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
-    <row r="8" spans="2:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -618,8 +691,11 @@
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="9" spans="2:4" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -627,6 +703,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>